<commit_message>
simulacion estanques excel dict
</commit_message>
<xml_diff>
--- a/docs/resultados_receta.xlsx
+++ b/docs/resultados_receta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>receta</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
   </si>
   <si>
     <t>B3</t>
@@ -404,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>4221689</v>
+        <v>1906477</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -437,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>2894676</v>
+        <v>180684</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -448,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>129222</v>
+        <v>1725793</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -459,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1197790</v>
+        <v>1143886</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -470,7 +467,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>2533013</v>
+        <v>1505228</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -481,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>4217573</v>
+        <v>401248</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -492,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>4115</v>
+        <v>18212</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -503,18 +500,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>13376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>1675299</v>
+        <v>744377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>